<commit_message>
Cambios en el notebook de masa
</commit_message>
<xml_diff>
--- a/data/raw/masa.xlsx
+++ b/data/raw/masa.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E54C06D-82C0-4724-B7F1-75AE7927804B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6C28CD-E2FD-4FE1-8821-478404D5473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$587</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5428" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5445" uniqueCount="627">
   <si>
     <t>CCM0001.M/2025</t>
   </si>
@@ -2267,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="G220" sqref="G220"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="T111" sqref="T111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8923,7 +8926,7 @@
         <v>8</v>
       </c>
       <c r="T110" s="2">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="111" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -25895,7 +25898,9 @@
       <c r="F394" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G394" s="2"/>
+      <c r="G394" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H394" s="3">
         <v>45671</v>
       </c>
@@ -26001,7 +26006,9 @@
       <c r="F397" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G397" s="2"/>
+      <c r="G397" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H397" s="3">
         <v>45671</v>
       </c>
@@ -26107,7 +26114,9 @@
       <c r="F400" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G400" s="2"/>
+      <c r="G400" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H400" s="3">
         <v>45671</v>
       </c>
@@ -26213,7 +26222,9 @@
       <c r="F403" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G403" s="2"/>
+      <c r="G403" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H403" s="3">
         <v>45671</v>
       </c>
@@ -26319,7 +26330,9 @@
       <c r="F406" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G406" s="2"/>
+      <c r="G406" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H406" s="3">
         <v>45671</v>
       </c>
@@ -26425,7 +26438,9 @@
       <c r="F409" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G409" s="2"/>
+      <c r="G409" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H409" s="3">
         <v>45671</v>
       </c>
@@ -26531,7 +26546,9 @@
       <c r="F412" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G412" s="2"/>
+      <c r="G412" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H412" s="3">
         <v>45671</v>
       </c>
@@ -26637,7 +26654,9 @@
       <c r="F415" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G415" s="2"/>
+      <c r="G415" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H415" s="3">
         <v>45671</v>
       </c>
@@ -26743,7 +26762,9 @@
       <c r="F418" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G418" s="2"/>
+      <c r="G418" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H418" s="3">
         <v>45671</v>
       </c>
@@ -26849,7 +26870,9 @@
       <c r="F421" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G421" s="2"/>
+      <c r="G421" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H421" s="3">
         <v>45671</v>
       </c>
@@ -26955,7 +26978,9 @@
       <c r="F424" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G424" s="2"/>
+      <c r="G424" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H424" s="3">
         <v>45671</v>
       </c>
@@ -27061,7 +27086,9 @@
       <c r="F427" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G427" s="2"/>
+      <c r="G427" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H427" s="3">
         <v>45671</v>
       </c>
@@ -31495,7 +31522,9 @@
       <c r="F549" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G549" s="2"/>
+      <c r="G549" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H549" s="3">
         <v>45700</v>
       </c>
@@ -31613,7 +31642,9 @@
       <c r="F551" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G551" s="2"/>
+      <c r="G551" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H551" s="3">
         <v>45714</v>
       </c>
@@ -31673,7 +31704,9 @@
       <c r="F552" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G552" s="2"/>
+      <c r="G552" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H552" s="3">
         <v>45714</v>
       </c>
@@ -31733,7 +31766,9 @@
       <c r="F553" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G553" s="2"/>
+      <c r="G553" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H553" s="3">
         <v>45700</v>
       </c>
@@ -31853,7 +31888,9 @@
       <c r="F555" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G555" s="2"/>
+      <c r="G555" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="H555" s="3">
         <v>45707</v>
       </c>
@@ -33629,6 +33666,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A587" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>